<commit_message>
commiting client admin integrated files
</commit_message>
<xml_diff>
--- a/src/test/resources/com/sirion/xls/Client Setup Admin Suite.xlsx
+++ b/src/test/resources/com/sirion/xls/Client Setup Admin Suite.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="27">
   <si>
     <t>TCID</t>
   </si>
@@ -85,19 +85,26 @@
     <t>DashboardSetup</t>
   </si>
   <si>
-    <t>Automation Supplier</t>
-  </si>
-  <si>
-    <t>aus</t>
-  </si>
-  <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Ajay Supplier</t>
+  </si>
+  <si>
+    <t>ajay</t>
+  </si>
+  <si>
+    <t>SKIP</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -496,15 +503,15 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.58203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="5.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -541,7 +548,9 @@
       <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="7"/>
+      <c r="D3" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -554,7 +563,9 @@
       <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="7"/>
+      <c r="D4" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -567,7 +578,9 @@
       <c r="C5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="7"/>
+      <c r="D5" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="E5" s="7"/>
     </row>
   </sheetData>
@@ -582,23 +595,23 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="7.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="5.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="7.58203125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="5.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -650,7 +663,9 @@
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
-      <c r="K2" s="3"/>
+      <c r="K2" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="L2" s="3"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -658,13 +673,13 @@
         <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>10</v>
@@ -673,10 +688,10 @@
         <v>9</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>10</v>
@@ -684,7 +699,9 @@
       <c r="J3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="2"/>
+      <c r="K3" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="L3" s="2"/>
     </row>
   </sheetData>
@@ -696,15 +713,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.58203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="5.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -728,7 +747,9 @@
       <c r="A2" s="5"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -736,12 +757,14 @@
         <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="E3" s="2"/>
     </row>
   </sheetData>
@@ -753,15 +776,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.58203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="5.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -785,7 +810,9 @@
       <c r="A2" s="5"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -793,12 +820,14 @@
         <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="E3" s="2"/>
     </row>
   </sheetData>

</xml_diff>